<commit_message>
update 2023/09/20 10:34:14:682 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC8F7ED-D378-47D3-8CFC-98F111004BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8A00D4-D4E8-433C-8071-566E14250277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -496,6 +496,14 @@
   </si>
   <si>
     <t>返回指定路径下，包含keyword的文件或文件夹的路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addfield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向struct列向量中添加字段</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -668,7 +676,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -683,22 +707,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -979,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -994,25 +1002,25 @@
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1023,8 +1031,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="10"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1033,7 +1041,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1045,10 +1053,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1059,8 +1067,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1069,7 +1077,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1081,8 +1089,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1093,8 +1101,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1103,8 +1111,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1113,430 +1121,440 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="2" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="7" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="2" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="2" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="3" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="2" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="2" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="2" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="10"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="13"/>
-      <c r="B22" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="14"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="3" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="2" t="s">
+    <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="2" t="s">
+    <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="2" t="s">
+    <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="2" t="s">
+    <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="13"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="3" t="s">
+    <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="3" t="s">
+    <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="12" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="13"/>
-      <c r="B34" s="7" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="13"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="2" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="13"/>
-      <c r="B36" s="7" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="13"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="13"/>
-      <c r="B38" s="7" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="14"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="2" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="12" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="3" t="s">
+      <c r="B41" s="12"/>
+      <c r="C41" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="2" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="13"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="3" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="13"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="13"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="2" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="13"/>
-      <c r="B45" s="15"/>
-      <c r="C45" s="2" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="13"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="3" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="13"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="14"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A33:A39"/>
-    <mergeCell ref="A40:A48"/>
-    <mergeCell ref="B40:B48"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A26:A32"/>
-    <mergeCell ref="B26:B32"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A17"/>
-    <mergeCell ref="A18:A25"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="A34:A40"/>
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="B41:B49"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2023/09/25 16:27:46:651 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8A00D4-D4E8-433C-8071-566E14250277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6E5AE-7B6B-49EA-A4EE-1DE2F24A03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -504,6 +504,14 @@
   </si>
   <si>
     <t>向struct列向量中添加字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>figureViewer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>图片拼接滚动查看</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -680,19 +688,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -705,6 +701,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -987,10 +995,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1017,10 +1025,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1031,8 +1039,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1049,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1053,10 +1061,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1067,8 +1075,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1085,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1089,8 +1097,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1101,8 +1109,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1111,8 +1119,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1121,8 +1129,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3" t="s">
         <v>118</v>
       </c>
@@ -1131,8 +1139,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1141,7 +1149,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1153,7 +1161,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1165,8 +1173,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1177,8 +1185,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1187,8 +1195,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1197,8 +1205,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
@@ -1207,10 +1215,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1221,8 +1229,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1231,8 +1239,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
@@ -1241,8 +1249,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1251,8 +1259,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1263,8 +1271,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="2" t="s">
         <v>59</v>
       </c>
@@ -1273,8 +1281,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2" t="s">
         <v>61</v>
       </c>
@@ -1283,8 +1291,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="3" t="s">
         <v>63</v>
       </c>
@@ -1293,10 +1301,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="3" t="s">
         <v>116</v>
       </c>
@@ -1305,8 +1313,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1315,8 +1323,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2" t="s">
         <v>68</v>
       </c>
@@ -1325,8 +1333,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="2" t="s">
         <v>70</v>
       </c>
@@ -1335,8 +1343,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="2" t="s">
         <v>71</v>
       </c>
@@ -1345,8 +1353,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="3" t="s">
         <v>73</v>
       </c>
@@ -1355,8 +1363,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="3" t="s">
         <v>75</v>
       </c>
@@ -1365,7 +1373,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="14" t="s">
         <v>77</v>
       </c>
       <c r="B34" s="6" t="s">
@@ -1379,8 +1387,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="12" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="9" t="s">
         <v>81</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1391,8 +1399,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="14"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="10"/>
       <c r="C36" s="2" t="s">
         <v>84</v>
       </c>
@@ -1401,8 +1409,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="12" t="s">
+      <c r="A37" s="15"/>
+      <c r="B37" s="9" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -1413,8 +1421,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="14"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="10"/>
       <c r="C38" s="2" t="s">
         <v>89</v>
       </c>
@@ -1423,8 +1431,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="12" t="s">
+      <c r="A39" s="15"/>
+      <c r="B39" s="9" t="s">
         <v>91</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -1435,126 +1443,136 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="11"/>
-      <c r="B40" s="14"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="17"/>
       <c r="C40" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="16"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="B41" s="12"/>
-      <c r="C41" s="3" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="10"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="2" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="15"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="10"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="3" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="3" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
+      <c r="C45" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="2" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="15"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="2" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="15"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="3" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="15"/>
+      <c r="B48" s="17"/>
+      <c r="C48" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="15"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="11"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="2" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A34:A41"/>
+    <mergeCell ref="A42:A50"/>
+    <mergeCell ref="B42:B50"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:B33"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="A19:A26"/>
-    <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A41:A49"/>
-    <mergeCell ref="B41:B49"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2023-11-23 16:23:01 by desktop-stc66qq
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LAB\MATLABUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6E5AE-7B6B-49EA-A4EE-1DE2F24A03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459AAA18-2F5B-46F6-81FF-1F7AC6B64375}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -512,6 +512,260 @@
   </si>
   <si>
     <t>图片拼接滚动查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deleteItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除指定路径下，包含keyword的文件或文件夹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>renameItem</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重命名指定路径下，包含keyword的文件或文件夹</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mNchoosek</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到数组data的nPool（&gt;=1)个元素的所有组合。可前接header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meanExcludeNaN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对矩阵中除NaN和Inf之外的元素求平均值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SEExcludeNaN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对矩阵中除NaN和Inf之外的元素求SE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mat2cellStr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将矩阵中的标量全部变成cell包起来的char格式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>excludeNaN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将矩阵中包含NaN/Inf的行或列删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对元素为数组的cell进行unique，且可以决定当不同cell存在相同元素时的保留选项。Simple:无视数组内元素的重复；largest set:只返回父集；minumum set:只返回子集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mUniqueCell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isCellByCol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mContrains</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以提供一个字符串数组，对其按照or/and的规则返回符合条件的字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据cell中元素的类型（默认某行或某列是同一类型），判断cell是否是按列分布的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>structSelect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从原始struct中选择特定字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addFieldToStruct</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可同时向struct中添加多个字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>structcat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将多个struct连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mCopyFields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将特定字段从A复制到B中（B为已存在的struct）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mKeepFields</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同structSelect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addLegend2Fig</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向图中指定位置放置legend，要求包含m*n个同样大小的子图</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alphaAxes</t>
+  </si>
+  <si>
+    <t>deleteLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定指定属性的值，将符合该值的线条删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getObjVal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对图中指定的对象设置透明度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定指定属性的值，获取符合该值的对象的其他属性值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定指定属性的值，获取符合该值的线条的其他属性值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>orderLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定指定属性的值，将符合该值的线条放在Axes的最上/最下面</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setAxes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置图像的特定属性值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setLine</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设定指定属性的值，对符合该值的线条的其他属性赋值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>setTile</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量设置标题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>att2AmpRatio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算衰减值对应的比例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auc_analysis</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入向量A和B，计算AUC值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>chi2test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>卡方检验</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>findWithinWindow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>找到特定时间窗口内的所有值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mAnovaCell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对cell(trialData)进行Anova</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mBootstrp</t>
+  </si>
+  <si>
+    <t>对cell或matrix进行bootstrp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dPrime</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入hit和correct reject求d'值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rsquare</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据拟合值计算R2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,7 +924,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -688,7 +942,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -703,18 +969,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -995,22 +1250,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="B27" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="135.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="30.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.75" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="149.875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="8" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>11</v>
       </c>
@@ -1024,11 +1279,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1038,9 +1293,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1048,8 +1303,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17"/>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1060,11 +1315,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1074,505 +1329,826 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="2" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
+      <c r="B9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="3" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="2" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="10"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="10"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="10"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="10"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="6" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10"/>
+      <c r="B20" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="6" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="9" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="2" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="10"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="10"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="10"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B32" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="2" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="3" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="9" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="2" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="2" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="3" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="11"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="3" t="s">
+      <c r="B48" s="12"/>
+      <c r="C48" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="2" t="s">
+    <row r="52" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="2" t="s">
+    <row r="53" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D53" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="2" t="s">
+    <row r="54" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D54" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="3" t="s">
+    <row r="55" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="3" t="s">
+    <row r="56" spans="1:4" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B57" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="9" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C58" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="2" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="10"/>
+      <c r="B59" s="14"/>
+      <c r="C59" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="9" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="10"/>
+      <c r="B60" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="2" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="10"/>
+      <c r="B61" s="14"/>
+      <c r="C61" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="9" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C62" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D62" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="2" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="2" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="11"/>
+      <c r="B64" s="14"/>
+      <c r="C64" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D64" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="3" t="s">
+      <c r="B65" s="12"/>
+      <c r="C65" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="2" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="3" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="3" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D68" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="15"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="2" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D69" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="2" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="10"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="3" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="10"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="15"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="2" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="2" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="10"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="11"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
+  <mergeCells count="18">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B5:B8"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="A5:A31"/>
+    <mergeCell ref="A32:A47"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A57:A64"/>
+    <mergeCell ref="A65:A82"/>
+    <mergeCell ref="B65:B82"/>
+    <mergeCell ref="B10:B19"/>
+    <mergeCell ref="B23:B31"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B32:B43"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="A48:A56"/>
+    <mergeCell ref="B48:B56"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2023/11/25 17:11:57:567 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC6E5AE-7B6B-49EA-A4EE-1DE2F24A03E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48206C40-1CEC-4B92-B02F-0A6B2B7774FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -263,14 +263,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>cwtMulti_5001_64_mex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>在GPU中计算小波变换结果，5001为数据时间上的点数，64为通道数，数据需要以[time,ch]的方式输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mGpucoder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -512,6 +504,30 @@
   </si>
   <si>
     <t>图片拼接滚动查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cwtAny</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>返回小波变换的原始结果，对任意trial数目和通道数目的数据，可以指定分隔数目以便进行GPU加速</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ft_removePath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>移除FieldTrip相关搜索路径，但是保留ft_defaults</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generateGradientColors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成一组渐变色rgb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -688,7 +704,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -701,18 +729,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -995,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1025,10 +1041,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1039,8 +1055,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1049,7 +1065,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1061,10 +1077,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1075,8 +1091,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="15"/>
-      <c r="B6" s="10"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="14"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1085,7 +1101,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1097,8 +1113,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="10"/>
+      <c r="B8" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1109,8 +1125,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="15"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="10"/>
+      <c r="B9" s="13"/>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1119,8 +1135,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="15"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1129,18 +1145,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15"/>
-      <c r="B11" s="17"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="14"/>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1149,7 +1165,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
+      <c r="A13" s="10"/>
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1161,7 +1177,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1173,8 +1189,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="10"/>
+      <c r="B15" s="12" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1185,8 +1201,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="17"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1195,8 +1211,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="17"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1205,8 +1221,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="10"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="14"/>
       <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
@@ -1215,10 +1231,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="12" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1229,8 +1245,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1239,8 +1255,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="17"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
@@ -1249,8 +1265,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="10"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1259,320 +1275,341 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="15"/>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="10"/>
+      <c r="B23" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="10"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="2" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="10"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="16"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
+      <c r="D28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="2" t="s">
+    </row>
+    <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="2" t="s">
+    <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="3" t="s">
+    <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="11"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="16"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="3" t="s">
+    <row r="34" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="B34" s="12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+      <c r="C34" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="D34" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10"/>
+      <c r="B36" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="9" t="s">
+      <c r="D36" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="2" t="s">
+    </row>
+    <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="10"/>
-      <c r="C36" s="2" t="s">
+    <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10"/>
+      <c r="B38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="15"/>
-      <c r="B37" s="9" t="s">
+      <c r="D38" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="10"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="10"/>
-      <c r="C38" s="2" t="s">
+    <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="C40" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="9" t="s">
+      <c r="D40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C39" s="3" t="s">
+    </row>
+    <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="17"/>
-      <c r="C40" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="16"/>
-      <c r="B41" s="10"/>
-      <c r="C41" s="2" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="B43" s="12"/>
+      <c r="C43" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="14" t="s">
+      <c r="D43" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="3" t="s">
+      <c r="D44" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="2" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="10"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="3" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="15"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="2" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="2" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="10"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="3" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="15"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="2" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="16"/>
-      <c r="B50" s="10"/>
-      <c r="C50" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="A42:A50"/>
-    <mergeCell ref="B42:B50"/>
-    <mergeCell ref="B8:B12"/>
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="B27:B33"/>
+  <mergeCells count="18">
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A18"/>
     <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A43:A52"/>
+    <mergeCell ref="B43:B52"/>
+    <mergeCell ref="B8:B12"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="B27:B33"/>
+    <mergeCell ref="A34:A42"/>
+    <mergeCell ref="B34:B35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2023-12-06 15:40:43 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48206C40-1CEC-4B92-B02F-0A6B2B7774FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76F6723A-10EF-4BE3-905D-38A8E9425722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,10 +495,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>向struct列向量中添加字段</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>figureViewer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -528,6 +524,10 @@
   </si>
   <si>
     <t>生成一组渐变色rgb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>向struct列向量中添加字段或修改某字段的值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -704,19 +704,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -729,6 +717,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1041,10 +1041,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1055,8 +1055,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="16"/>
-      <c r="B3" s="14"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1065,7 +1065,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="6" t="s">
         <v>31</v>
       </c>
@@ -1077,10 +1077,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1091,8 +1091,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="14"/>
+      <c r="A6" s="15"/>
+      <c r="B6" s="10"/>
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1101,7 +1101,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
@@ -1113,8 +1113,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1125,8 +1125,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1135,8 +1135,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="13"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1145,18 +1145,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="13"/>
+      <c r="A11" s="15"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="3" t="s">
         <v>116</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="14"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1165,7 +1165,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="6" t="s">
         <v>29</v>
       </c>
@@ -1177,7 +1177,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="6" t="s">
         <v>34</v>
       </c>
@@ -1189,8 +1189,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="10"/>
-      <c r="B15" s="12" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="9" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1201,8 +1201,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="10"/>
-      <c r="B16" s="13"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="17"/>
       <c r="C16" s="2" t="s">
         <v>40</v>
       </c>
@@ -1211,8 +1211,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="10"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="2" t="s">
         <v>42</v>
       </c>
@@ -1221,8 +1221,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="10"/>
       <c r="C18" s="3" t="s">
         <v>44</v>
       </c>
@@ -1231,10 +1231,10 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="9" t="s">
         <v>47</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1245,8 +1245,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
@@ -1255,8 +1255,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="2" t="s">
         <v>52</v>
       </c>
@@ -1265,8 +1265,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="10"/>
-      <c r="B22" s="14"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="3" t="s">
         <v>54</v>
       </c>
@@ -1275,20 +1275,20 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="10"/>
-      <c r="B23" s="12" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="10"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="17"/>
       <c r="C24" s="2" t="s">
         <v>57</v>
       </c>
@@ -1297,8 +1297,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10"/>
-      <c r="B25" s="13"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="17"/>
       <c r="C25" s="2" t="s">
         <v>59</v>
       </c>
@@ -1307,8 +1307,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="14"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="10"/>
       <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
@@ -1317,10 +1317,10 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="3" t="s">
         <v>114</v>
       </c>
@@ -1329,8 +1329,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="17"/>
       <c r="C28" s="2" t="s">
         <v>64</v>
       </c>
@@ -1339,8 +1339,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="10"/>
-      <c r="B29" s="13"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="17"/>
       <c r="C29" s="2" t="s">
         <v>66</v>
       </c>
@@ -1349,8 +1349,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="10"/>
-      <c r="B30" s="13"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="2" t="s">
         <v>68</v>
       </c>
@@ -1359,8 +1359,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="2" t="s">
         <v>69</v>
       </c>
@@ -1369,8 +1369,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="17"/>
       <c r="C32" s="3" t="s">
         <v>71</v>
       </c>
@@ -1379,8 +1379,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="11"/>
-      <c r="B33" s="14"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="3" t="s">
         <v>73</v>
       </c>
@@ -1389,10 +1389,10 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1403,18 +1403,18 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="10"/>
-      <c r="B35" s="14"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="10"/>
       <c r="C35" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="10"/>
-      <c r="B36" s="12" t="s">
+      <c r="A36" s="15"/>
+      <c r="B36" s="9" t="s">
         <v>79</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1425,8 +1425,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="10"/>
-      <c r="B37" s="14"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="10"/>
       <c r="C37" s="2" t="s">
         <v>82</v>
       </c>
@@ -1435,8 +1435,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="10"/>
-      <c r="B38" s="12" t="s">
+      <c r="A38" s="15"/>
+      <c r="B38" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -1447,8 +1447,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="10"/>
-      <c r="B39" s="14"/>
+      <c r="A39" s="15"/>
+      <c r="B39" s="10"/>
       <c r="C39" s="2" t="s">
         <v>87</v>
       </c>
@@ -1457,8 +1457,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="10"/>
-      <c r="B40" s="12" t="s">
+      <c r="A40" s="15"/>
+      <c r="B40" s="9" t="s">
         <v>89</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1469,18 +1469,18 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="10"/>
-      <c r="B41" s="13"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="17"/>
       <c r="C41" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>119</v>
-      </c>
     </row>
     <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="11"/>
-      <c r="B42" s="14"/>
+      <c r="A42" s="16"/>
+      <c r="B42" s="10"/>
       <c r="C42" s="2" t="s">
         <v>92</v>
       </c>
@@ -1489,10 +1489,10 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="12"/>
+      <c r="B43" s="9"/>
       <c r="C43" s="3" t="s">
         <v>95</v>
       </c>
@@ -1501,8 +1501,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="10"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="17"/>
       <c r="C44" s="3" t="s">
         <v>96</v>
       </c>
@@ -1511,8 +1511,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="10"/>
-      <c r="B45" s="13"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="17"/>
       <c r="C45" s="3" t="s">
         <v>99</v>
       </c>
@@ -1521,8 +1521,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="13"/>
+      <c r="A46" s="15"/>
+      <c r="B46" s="17"/>
       <c r="C46" s="3" t="s">
         <v>101</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="10"/>
-      <c r="B47" s="13"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="17"/>
       <c r="C47" s="2" t="s">
         <v>103</v>
       </c>
@@ -1541,8 +1541,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" s="10"/>
-      <c r="B48" s="13"/>
+      <c r="A48" s="15"/>
+      <c r="B48" s="17"/>
       <c r="C48" s="2" t="s">
         <v>105</v>
       </c>
@@ -1551,8 +1551,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="10"/>
-      <c r="B49" s="13"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="3" t="s">
         <v>107</v>
       </c>
@@ -1561,8 +1561,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="10"/>
-      <c r="B50" s="13"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="17"/>
       <c r="C50" s="2" t="s">
         <v>109</v>
       </c>
@@ -1571,18 +1571,18 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="10"/>
-      <c r="B51" s="13"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="17"/>
       <c r="C51" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>125</v>
-      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="11"/>
-      <c r="B52" s="14"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="10"/>
       <c r="C52" s="2" t="s">
         <v>111</v>
       </c>
@@ -1592,12 +1592,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A18"/>
-    <mergeCell ref="A19:A26"/>
-    <mergeCell ref="B23:B26"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="B43:B52"/>
     <mergeCell ref="B8:B12"/>
@@ -1610,6 +1604,12 @@
     <mergeCell ref="B27:B33"/>
     <mergeCell ref="A34:A42"/>
     <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A18"/>
+    <mergeCell ref="A19:A26"/>
+    <mergeCell ref="B23:B26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2025-04-29 13:25:50 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD2A058-B738-4814-8447-8FD4301A21FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D363EBA5-1FF0-4FE1-9458-945338632A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -906,6 +906,14 @@
   </si>
   <si>
     <t>click train生成的通用函数，可以生成任意结构的click train</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tonegen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成纯音/复杂声</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1112,19 +1120,28 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1134,15 +1151,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1425,10 +1433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D98" sqref="D98"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1455,10 +1463,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="22" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1469,8 +1477,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="20"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1479,7 +1487,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1491,10 +1499,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="22" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1505,8 +1513,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="26"/>
-      <c r="B6" s="21"/>
+      <c r="A6" s="20"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="9" t="s">
         <v>125</v>
       </c>
@@ -1515,8 +1523,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="26"/>
-      <c r="B7" s="21"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="23"/>
       <c r="C7" s="9" t="s">
         <v>126</v>
       </c>
@@ -1525,9 +1533,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="26"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="9" t="s">
+      <c r="A8" s="20"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="3" t="s">
         <v>196</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1535,9 +1543,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="9" t="s">
+      <c r="A9" s="20"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="3" t="s">
         <v>198</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1545,8 +1553,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="26"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
@@ -1555,7 +1563,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
@@ -1567,8 +1575,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="26"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="20"/>
+      <c r="B12" s="22" t="s">
         <v>19</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1579,8 +1587,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="26"/>
-      <c r="B13" s="21"/>
+      <c r="A13" s="20"/>
+      <c r="B13" s="23"/>
       <c r="C13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1589,8 +1597,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="26"/>
-      <c r="B14" s="21"/>
+      <c r="A14" s="20"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1599,8 +1607,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="21"/>
+      <c r="A15" s="20"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="3" t="s">
         <v>173</v>
       </c>
@@ -1609,8 +1617,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="26"/>
-      <c r="B16" s="21"/>
+      <c r="A16" s="20"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="3" t="s">
         <v>107</v>
       </c>
@@ -1619,8 +1627,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="26"/>
-      <c r="B17" s="21"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="9" t="s">
         <v>130</v>
       </c>
@@ -1629,8 +1637,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="26"/>
-      <c r="B18" s="21"/>
+      <c r="A18" s="20"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="9" t="s">
         <v>138</v>
       </c>
@@ -1639,8 +1647,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="26"/>
-      <c r="B19" s="21"/>
+      <c r="A19" s="20"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="9" t="s">
         <v>134</v>
       </c>
@@ -1649,8 +1657,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="26"/>
-      <c r="B20" s="21"/>
+      <c r="A20" s="20"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="9" t="s">
         <v>136</v>
       </c>
@@ -1659,9 +1667,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="26"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="9" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="3" t="s">
         <v>132</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -1669,8 +1677,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="26"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1679,8 +1687,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
-      <c r="B23" s="19" t="s">
+      <c r="A23" s="20"/>
+      <c r="B23" s="22" t="s">
         <v>28</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1691,8 +1699,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
-      <c r="B24" s="20"/>
+      <c r="A24" s="20"/>
+      <c r="B24" s="24"/>
       <c r="C24" s="2" t="s">
         <v>127</v>
       </c>
@@ -1701,8 +1709,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="22" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -1713,8 +1721,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
-      <c r="B26" s="20"/>
+      <c r="A26" s="20"/>
+      <c r="B26" s="24"/>
       <c r="C26" s="2" t="s">
         <v>34</v>
       </c>
@@ -1723,8 +1731,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
-      <c r="B27" s="19" t="s">
+      <c r="A27" s="20"/>
+      <c r="B27" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1735,8 +1743,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
-      <c r="B28" s="21"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="23"/>
       <c r="C28" s="2" t="s">
         <v>39</v>
       </c>
@@ -1745,8 +1753,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
-      <c r="B29" s="21"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="23"/>
       <c r="C29" s="2" t="s">
         <v>40</v>
       </c>
@@ -1755,8 +1763,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="26"/>
-      <c r="B30" s="21"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="23"/>
       <c r="C30" s="2" t="s">
         <v>120</v>
       </c>
@@ -1765,8 +1773,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="26"/>
-      <c r="B31" s="21"/>
+      <c r="A31" s="20"/>
+      <c r="B31" s="23"/>
       <c r="C31" s="2" t="s">
         <v>122</v>
       </c>
@@ -1775,8 +1783,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="26"/>
-      <c r="B32" s="21"/>
+      <c r="A32" s="20"/>
+      <c r="B32" s="23"/>
       <c r="C32" s="2" t="s">
         <v>118</v>
       </c>
@@ -1785,8 +1793,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="26"/>
-      <c r="B33" s="21"/>
+      <c r="A33" s="20"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="2" t="s">
         <v>116</v>
       </c>
@@ -1795,8 +1803,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="26"/>
-      <c r="B34" s="21"/>
+      <c r="A34" s="20"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="2" t="s">
         <v>114</v>
       </c>
@@ -1805,8 +1813,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="27"/>
-      <c r="B35" s="20"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="3" t="s">
         <v>42</v>
       </c>
@@ -1815,10 +1823,10 @@
       </c>
     </row>
     <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="22" t="s">
         <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -1829,8 +1837,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="26"/>
-      <c r="B37" s="21"/>
+      <c r="A37" s="20"/>
+      <c r="B37" s="23"/>
       <c r="C37" s="2" t="s">
         <v>48</v>
       </c>
@@ -1839,8 +1847,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26"/>
-      <c r="B38" s="21"/>
+      <c r="A38" s="20"/>
+      <c r="B38" s="23"/>
       <c r="C38" s="2" t="s">
         <v>50</v>
       </c>
@@ -1849,8 +1857,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26"/>
-      <c r="B39" s="21"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="23"/>
       <c r="C39" s="2" t="s">
         <v>157</v>
       </c>
@@ -1859,8 +1867,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26"/>
-      <c r="B40" s="21"/>
+      <c r="A40" s="20"/>
+      <c r="B40" s="23"/>
       <c r="C40" s="2" t="s">
         <v>159</v>
       </c>
@@ -1869,8 +1877,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="26"/>
-      <c r="B41" s="21"/>
+      <c r="A41" s="20"/>
+      <c r="B41" s="23"/>
       <c r="C41" s="2" t="s">
         <v>161</v>
       </c>
@@ -1879,8 +1887,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="26"/>
-      <c r="B42" s="21"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="23"/>
       <c r="C42" s="2" t="s">
         <v>165</v>
       </c>
@@ -1889,8 +1897,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="26"/>
-      <c r="B43" s="21"/>
+      <c r="A43" s="20"/>
+      <c r="B43" s="23"/>
       <c r="C43" s="2" t="s">
         <v>167</v>
       </c>
@@ -1899,8 +1907,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="26"/>
-      <c r="B44" s="21"/>
+      <c r="A44" s="20"/>
+      <c r="B44" s="23"/>
       <c r="C44" s="2" t="s">
         <v>169</v>
       </c>
@@ -1909,8 +1917,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="26"/>
-      <c r="B45" s="21"/>
+      <c r="A45" s="20"/>
+      <c r="B45" s="23"/>
       <c r="C45" s="2" t="s">
         <v>171</v>
       </c>
@@ -1919,8 +1927,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="26"/>
-      <c r="B46" s="21"/>
+      <c r="A46" s="20"/>
+      <c r="B46" s="23"/>
       <c r="C46" s="3" t="s">
         <v>163</v>
       </c>
@@ -1929,8 +1937,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="26"/>
-      <c r="B47" s="20"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="24"/>
       <c r="C47" s="3" t="s">
         <v>52</v>
       </c>
@@ -1939,8 +1947,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="26"/>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="20"/>
+      <c r="B48" s="22" t="s">
         <v>54</v>
       </c>
       <c r="C48" s="16" t="s">
@@ -1951,8 +1959,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="26"/>
-      <c r="B49" s="21"/>
+      <c r="A49" s="20"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="3" t="s">
         <v>184</v>
       </c>
@@ -1961,8 +1969,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="26"/>
-      <c r="B50" s="21"/>
+      <c r="A50" s="20"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="16" t="s">
         <v>185</v>
       </c>
@@ -1971,8 +1979,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="26"/>
-      <c r="B51" s="20"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="24"/>
       <c r="C51" s="3" t="s">
         <v>56</v>
       </c>
@@ -1981,8 +1989,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="26"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="20"/>
+      <c r="B52" s="22" t="s">
         <v>186</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -1993,8 +2001,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="26"/>
-      <c r="B53" s="21"/>
+      <c r="A53" s="20"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="9" t="s">
         <v>189</v>
       </c>
@@ -2003,8 +2011,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="21"/>
+      <c r="A54" s="20"/>
+      <c r="B54" s="23"/>
       <c r="C54" s="9" t="s">
         <v>191</v>
       </c>
@@ -2013,8 +2021,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="27"/>
-      <c r="B55" s="20"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="24"/>
       <c r="C55" s="9" t="s">
         <v>187</v>
       </c>
@@ -2023,10 +2031,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="25" t="s">
+      <c r="A56" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="19"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="3" t="s">
         <v>105</v>
       </c>
@@ -2035,8 +2043,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="26"/>
-      <c r="B57" s="21"/>
+      <c r="A57" s="20"/>
+      <c r="B57" s="23"/>
       <c r="C57" s="3" t="s">
         <v>110</v>
       </c>
@@ -2045,8 +2053,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="26"/>
-      <c r="B58" s="21"/>
+      <c r="A58" s="20"/>
+      <c r="B58" s="23"/>
       <c r="C58" s="3" t="s">
         <v>112</v>
       </c>
@@ -2055,8 +2063,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="26"/>
-      <c r="B59" s="21"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="23"/>
       <c r="C59" s="2" t="s">
         <v>59</v>
       </c>
@@ -2065,8 +2073,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="26"/>
-      <c r="B60" s="21"/>
+      <c r="A60" s="20"/>
+      <c r="B60" s="23"/>
       <c r="C60" s="2" t="s">
         <v>175</v>
       </c>
@@ -2075,8 +2083,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="26"/>
-      <c r="B61" s="21"/>
+      <c r="A61" s="20"/>
+      <c r="B61" s="23"/>
       <c r="C61" s="3" t="s">
         <v>176</v>
       </c>
@@ -2085,8 +2093,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="26"/>
-      <c r="B62" s="21"/>
+      <c r="A62" s="20"/>
+      <c r="B62" s="23"/>
       <c r="C62" s="2" t="s">
         <v>61</v>
       </c>
@@ -2095,8 +2103,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="26"/>
-      <c r="B63" s="21"/>
+      <c r="A63" s="20"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="2" t="s">
         <v>62</v>
       </c>
@@ -2105,8 +2113,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="26"/>
-      <c r="B64" s="21"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="2" t="s">
         <v>63</v>
       </c>
@@ -2115,8 +2123,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="26"/>
-      <c r="B65" s="21"/>
+      <c r="A65" s="20"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="3" t="s">
         <v>65</v>
       </c>
@@ -2125,8 +2133,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="26"/>
-      <c r="B66" s="21"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="3" t="s">
         <v>67</v>
       </c>
@@ -2135,8 +2143,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="27"/>
-      <c r="B67" s="20"/>
+      <c r="A67" s="21"/>
+      <c r="B67" s="24"/>
       <c r="C67" s="3" t="s">
         <v>177</v>
       </c>
@@ -2145,7 +2153,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="25" t="s">
+      <c r="A68" s="19" t="s">
         <v>69</v>
       </c>
       <c r="B68" s="6" t="s">
@@ -2159,8 +2167,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="26"/>
-      <c r="B69" s="19" t="s">
+      <c r="A69" s="20"/>
+      <c r="B69" s="22" t="s">
         <v>73</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2171,8 +2179,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="26"/>
-      <c r="B70" s="20"/>
+      <c r="A70" s="20"/>
+      <c r="B70" s="24"/>
       <c r="C70" s="2" t="s">
         <v>76</v>
       </c>
@@ -2181,8 +2189,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="26"/>
-      <c r="B71" s="19" t="s">
+      <c r="A71" s="20"/>
+      <c r="B71" s="22" t="s">
         <v>78</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2193,8 +2201,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="26"/>
-      <c r="B72" s="20"/>
+      <c r="A72" s="20"/>
+      <c r="B72" s="24"/>
       <c r="C72" s="2" t="s">
         <v>81</v>
       </c>
@@ -2203,8 +2211,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="26"/>
-      <c r="B73" s="19" t="s">
+      <c r="A73" s="20"/>
+      <c r="B73" s="22" t="s">
         <v>83</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -2215,8 +2223,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="26"/>
-      <c r="B74" s="21"/>
+      <c r="A74" s="20"/>
+      <c r="B74" s="23"/>
       <c r="C74" s="2" t="s">
         <v>108</v>
       </c>
@@ -2225,8 +2233,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="26"/>
-      <c r="B75" s="21"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="23"/>
       <c r="C75" s="2" t="s">
         <v>215</v>
       </c>
@@ -2235,8 +2243,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="27"/>
-      <c r="B76" s="20"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="24"/>
       <c r="C76" s="2" t="s">
         <v>86</v>
       </c>
@@ -2245,10 +2253,10 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="25" t="s">
+      <c r="A77" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="19"/>
+      <c r="B77" s="22"/>
       <c r="C77" s="3" t="s">
         <v>89</v>
       </c>
@@ -2257,8 +2265,8 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="26"/>
-      <c r="B78" s="21"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="23"/>
       <c r="C78" s="9" t="s">
         <v>179</v>
       </c>
@@ -2267,8 +2275,8 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="26"/>
-      <c r="B79" s="21"/>
+      <c r="A79" s="20"/>
+      <c r="B79" s="23"/>
       <c r="C79" s="2" t="s">
         <v>90</v>
       </c>
@@ -2277,8 +2285,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="26"/>
-      <c r="B80" s="21"/>
+      <c r="A80" s="20"/>
+      <c r="B80" s="23"/>
       <c r="C80" s="10" t="s">
         <v>92</v>
       </c>
@@ -2287,8 +2295,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="26"/>
-      <c r="B81" s="21"/>
+      <c r="A81" s="20"/>
+      <c r="B81" s="23"/>
       <c r="C81" s="3" t="s">
         <v>93</v>
       </c>
@@ -2297,8 +2305,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="26"/>
-      <c r="B82" s="21"/>
+      <c r="A82" s="20"/>
+      <c r="B82" s="23"/>
       <c r="C82" s="2" t="s">
         <v>95</v>
       </c>
@@ -2307,8 +2315,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="26"/>
-      <c r="B83" s="21"/>
+      <c r="A83" s="20"/>
+      <c r="B83" s="23"/>
       <c r="C83" s="2" t="s">
         <v>97</v>
       </c>
@@ -2317,8 +2325,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="26"/>
-      <c r="B84" s="21"/>
+      <c r="A84" s="20"/>
+      <c r="B84" s="23"/>
       <c r="C84" s="3" t="s">
         <v>99</v>
       </c>
@@ -2327,8 +2335,8 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="26"/>
-      <c r="B85" s="21"/>
+      <c r="A85" s="20"/>
+      <c r="B85" s="23"/>
       <c r="C85" s="3" t="s">
         <v>100</v>
       </c>
@@ -2337,8 +2345,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="26"/>
-      <c r="B86" s="21"/>
+      <c r="A86" s="20"/>
+      <c r="B86" s="23"/>
       <c r="C86" s="2" t="s">
         <v>140</v>
       </c>
@@ -2347,8 +2355,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="26"/>
-      <c r="B87" s="21"/>
+      <c r="A87" s="20"/>
+      <c r="B87" s="23"/>
       <c r="C87" s="2" t="s">
         <v>152</v>
       </c>
@@ -2357,8 +2365,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="26"/>
-      <c r="B88" s="21"/>
+      <c r="A88" s="20"/>
+      <c r="B88" s="23"/>
       <c r="C88" s="2" t="s">
         <v>142</v>
       </c>
@@ -2367,8 +2375,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="26"/>
-      <c r="B89" s="21"/>
+      <c r="A89" s="20"/>
+      <c r="B89" s="23"/>
       <c r="C89" s="2" t="s">
         <v>143</v>
       </c>
@@ -2377,8 +2385,8 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="26"/>
-      <c r="B90" s="21"/>
+      <c r="A90" s="20"/>
+      <c r="B90" s="23"/>
       <c r="C90" s="2" t="s">
         <v>150</v>
       </c>
@@ -2387,8 +2395,8 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="26"/>
-      <c r="B91" s="21"/>
+      <c r="A91" s="20"/>
+      <c r="B91" s="23"/>
       <c r="C91" s="2" t="s">
         <v>145</v>
       </c>
@@ -2397,8 +2405,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="26"/>
-      <c r="B92" s="21"/>
+      <c r="A92" s="20"/>
+      <c r="B92" s="23"/>
       <c r="C92" s="2" t="s">
         <v>154</v>
       </c>
@@ -2407,8 +2415,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="26"/>
-      <c r="B93" s="21"/>
+      <c r="A93" s="20"/>
+      <c r="B93" s="23"/>
       <c r="C93" s="2" t="s">
         <v>146</v>
       </c>
@@ -2417,8 +2425,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="26"/>
-      <c r="B94" s="21"/>
+      <c r="A94" s="20"/>
+      <c r="B94" s="23"/>
       <c r="C94" s="2" t="s">
         <v>181</v>
       </c>
@@ -2427,8 +2435,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="27"/>
-      <c r="B95" s="20"/>
+      <c r="A95" s="21"/>
+      <c r="B95" s="24"/>
       <c r="C95" s="2" t="s">
         <v>102</v>
       </c>
@@ -2436,11 +2444,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="17" t="s">
+    <row r="96" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="B96" s="18" t="s">
+      <c r="B96" s="22" t="s">
         <v>218</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -2450,31 +2458,52 @@
         <v>220</v>
       </c>
     </row>
-    <row r="98" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="13" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="21"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A98" s="18"/>
+      <c r="B98" s="17"/>
+    </row>
+    <row r="99" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A99" s="13" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="14"/>
-      <c r="B99" s="12" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="14"/>
+      <c r="B100" s="12" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="11"/>
-      <c r="B100" s="12" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="11"/>
+      <c r="B101" s="12" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="15"/>
-      <c r="B101" s="12" t="s">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="15"/>
+      <c r="B102" s="12" t="s">
         <v>211</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A35"/>
+    <mergeCell ref="B23:B24"/>
     <mergeCell ref="A68:A76"/>
     <mergeCell ref="A77:A95"/>
     <mergeCell ref="B77:B95"/>
@@ -2490,11 +2519,6 @@
     <mergeCell ref="A36:A55"/>
     <mergeCell ref="B52:B55"/>
     <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A35"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 20250630 by xhx
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D363EBA5-1FF0-4FE1-9458-945338632A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C841C3-9A06-4861-B520-590B18E2C019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,18 +188,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>在矩阵指定行插入零行向量</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mMapminmax</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>replaceVal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>对标量输入x，如果满足条件val0则将其替换为val并返回</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -769,34 +770,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>spike</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>calLatency</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据spike time计算latency，精确到spike时刻</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>calFR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据spike time计算窗口内平均发放率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>calPSTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据spike time返回PSTH</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mHist</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -809,14 +782,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>calchMean/calchErr</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>计算trialsData的通道mean/通道standard error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>cutData</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -914,6 +879,138 @@
   </si>
   <si>
     <t>生成纯音/复杂声</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calchMean/calchErr/calchFunc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算trialsData的通道mean/通道standard error，calchFunc可以指定任意函数对trialsData进行计算</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mErrorFcn/mErrorFcnEmpty</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrorHandler通用函数，分别返回nan和[]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在矩阵指定行之前插入零行向量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>replaceVal/replaceValMat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vectorShift</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将向量向头/尾移动并补零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mFilter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零相移带通滤波和陷波</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>+mstat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可返回常见统计检验函数的effect size和BF10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exportcolorbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出colorbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mExportgraphics</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同时导出多个axes，可重叠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addSpecialTicks</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加特定数值位置的tick label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>addWaveErr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加shaded errorbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>copyaxes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将指定axes中的内容复制到另一个axes中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mColorbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在不改变axes大小的情况下添加colorbar</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>generateGradientColors</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生成指定颜色到白色的渐变色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>syncXY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将x和y的范围设置成一致</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>slanCM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boxplotGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>常用的colormap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分组boxplot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1084,7 +1181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1126,22 +1223,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1153,6 +1250,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1433,17 +1534,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D102"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D108" sqref="D108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.77734375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="149.88671875" style="2" customWidth="1"/>
     <col min="5" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1466,7 +1567,7 @@
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1478,7 +1579,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="26"/>
-      <c r="B3" s="24"/>
+      <c r="B3" s="21"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1499,10 +1600,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="20" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1513,288 +1614,288 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="24"/>
       <c r="C6" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="28"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="28"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
+      <c r="B13" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="28"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="28"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="28"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="28"/>
+      <c r="B24" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="9" t="s">
+      <c r="D25" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="22" t="s">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="22" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="28"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="28"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="28"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="28"/>
+      <c r="B33" s="24"/>
       <c r="C33" s="2" t="s">
         <v>116</v>
       </c>
@@ -1803,8 +1904,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="23"/>
+      <c r="A34" s="28"/>
+      <c r="B34" s="24"/>
       <c r="C34" s="2" t="s">
         <v>114</v>
       </c>
@@ -1813,712 +1914,821 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="21"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="24"/>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="28"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="23"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="B38" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="20" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="19" t="s">
+      <c r="C39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="D39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="28"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="20"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="2" t="s">
+    <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="20"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="2" t="s">
+    <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="28"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="28"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="28"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="28"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="28"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="28"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="28"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="28"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="28"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="28"/>
+      <c r="B52" s="21"/>
+      <c r="C52" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="D52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="20"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="20"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="20"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="20"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="20"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="20"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="20"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="20"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="20"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="3" t="s">
+    <row r="53" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="28"/>
+      <c r="B53" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="C53" s="16" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="20"/>
-      <c r="B48" s="22" t="s">
+      <c r="D53" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="28"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="28"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="28"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C48" s="16" t="s">
+      <c r="D56" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="20"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="20"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="20"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="3" t="s">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="B57" s="20"/>
+      <c r="C57" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="28"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="28"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="28"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="20"/>
-      <c r="B52" s="22" t="s">
+      <c r="D60" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="28"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="28"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="28"/>
+      <c r="B63" s="24"/>
+      <c r="C63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="20"/>
-      <c r="B53" s="23"/>
-      <c r="C53" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="20"/>
-      <c r="B54" s="23"/>
-      <c r="C54" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="21"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="20"/>
-      <c r="B57" s="23"/>
-      <c r="C57" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="20"/>
-      <c r="B58" s="23"/>
-      <c r="C58" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="20"/>
-      <c r="B59" s="23"/>
-      <c r="C59" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D59" s="2" t="s">
+    </row>
+    <row r="64" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="28"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="20"/>
-      <c r="B60" s="23"/>
-      <c r="C60" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="20"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="20"/>
-      <c r="B62" s="23"/>
-      <c r="C62" s="2" t="s">
+      <c r="D64" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="28"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="20"/>
-      <c r="B63" s="23"/>
-      <c r="C63" s="2" t="s">
+      <c r="D65" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="20"/>
-      <c r="B64" s="23"/>
-      <c r="C64" s="2" t="s">
+    </row>
+    <row r="66" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="28"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D64" s="2" t="s">
+      <c r="D66" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20"/>
-      <c r="B65" s="23"/>
-      <c r="C65" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="20"/>
-      <c r="B66" s="23"/>
-      <c r="C66" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="67" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="21"/>
+      <c r="A67" s="28"/>
       <c r="B67" s="24"/>
       <c r="C67" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="28"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="28"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="23"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="28"/>
+      <c r="B72" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="28"/>
+      <c r="B73" s="21"/>
+      <c r="C73" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="28"/>
+      <c r="B74" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="28"/>
+      <c r="B75" s="21"/>
+      <c r="C75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="28"/>
+      <c r="B76" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="28"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="28"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="23"/>
+      <c r="B79" s="21"/>
+      <c r="C79" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="C80" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="28"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="20"/>
-      <c r="B69" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="20"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="20"/>
-      <c r="B71" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="20"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="20"/>
-      <c r="B73" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="20"/>
-      <c r="B74" s="23"/>
-      <c r="C74" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="20"/>
-      <c r="B75" s="23"/>
-      <c r="C75" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="21"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="19" t="s">
+    <row r="82" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="28"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B77" s="22"/>
-      <c r="C77" s="3" t="s">
+      <c r="D82" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D77" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="20"/>
-      <c r="B78" s="23"/>
-      <c r="C78" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="20"/>
-      <c r="B79" s="23"/>
-      <c r="C79" s="2" t="s">
+    </row>
+    <row r="83" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="28"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D83" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="28"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="20"/>
-      <c r="B80" s="23"/>
-      <c r="C80" s="10" t="s">
+      <c r="D84" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" s="20"/>
-      <c r="B81" s="23"/>
-      <c r="C81" s="3" t="s">
+    </row>
+    <row r="85" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="28"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="28"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" s="20"/>
-      <c r="B82" s="23"/>
-      <c r="C82" s="2" t="s">
+    <row r="87" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="28"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="20"/>
-      <c r="B83" s="23"/>
-      <c r="C83" s="2" t="s">
+    <row r="88" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="28"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D88" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="28"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" s="20"/>
-      <c r="B84" s="23"/>
-      <c r="C84" s="3" t="s">
+      <c r="D89" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D84" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" s="20"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" s="20"/>
-      <c r="B86" s="23"/>
-      <c r="C86" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" s="20"/>
-      <c r="B87" s="23"/>
-      <c r="C87" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="20"/>
-      <c r="B88" s="23"/>
-      <c r="C88" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A89" s="20"/>
-      <c r="B89" s="23"/>
-      <c r="C89" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A90" s="20"/>
-      <c r="B90" s="23"/>
+    </row>
+    <row r="90" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="28"/>
+      <c r="B90" s="24"/>
       <c r="C90" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="28"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="28"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="28"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="28"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A91" s="20"/>
-      <c r="B91" s="23"/>
-      <c r="C91" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="20"/>
-      <c r="B92" s="23"/>
-      <c r="C92" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="20"/>
-      <c r="B93" s="23"/>
-      <c r="C93" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" s="20"/>
-      <c r="B94" s="23"/>
-      <c r="C94" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="D94" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" s="21"/>
+    <row r="95" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="28"/>
       <c r="B95" s="24"/>
       <c r="C95" s="2" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="19" t="s">
-        <v>217</v>
-      </c>
-      <c r="B96" s="22" t="s">
-        <v>218</v>
-      </c>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="28"/>
+      <c r="B96" s="24"/>
       <c r="C96" s="2" t="s">
-        <v>219</v>
+        <v>141</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="21"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="28"/>
       <c r="B97" s="24"/>
       <c r="C97" s="2" t="s">
-        <v>221</v>
+        <v>148</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="18"/>
-      <c r="B98" s="17"/>
-    </row>
-    <row r="99" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="28"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="28"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="28"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="28"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="28"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="28"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="28"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="28"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="23"/>
+      <c r="B106" s="21"/>
+      <c r="C106" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B107" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D107" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="14"/>
-      <c r="B100" s="12" t="s">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="23"/>
+      <c r="B108" s="21"/>
+      <c r="C108" s="2" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A101" s="11"/>
-      <c r="B101" s="12" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="15"/>
-      <c r="B102" s="12" t="s">
+      <c r="D108" s="2" t="s">
         <v>211</v>
       </c>
     </row>
+    <row r="109" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A109" s="18"/>
+      <c r="B109" s="17"/>
+    </row>
+    <row r="110" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A110" s="13" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="14"/>
+      <c r="B111" s="12" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="11"/>
+      <c r="B112" s="12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" s="15"/>
+      <c r="B113" s="12" t="s">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="A96:A97"/>
+  <mergeCells count="21">
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A38:A56"/>
+    <mergeCell ref="B80:B106"/>
+    <mergeCell ref="A80:A106"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="A57:A70"/>
+    <mergeCell ref="B57:B70"/>
+    <mergeCell ref="B107:B108"/>
+    <mergeCell ref="A107:A108"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B5:B11"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A35"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A68:A76"/>
-    <mergeCell ref="A77:A95"/>
-    <mergeCell ref="B77:B95"/>
-    <mergeCell ref="B12:B22"/>
-    <mergeCell ref="B27:B35"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B76"/>
-    <mergeCell ref="B36:B47"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A56:A67"/>
-    <mergeCell ref="B56:B67"/>
-    <mergeCell ref="A36:A55"/>
-    <mergeCell ref="B52:B55"/>
-    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A5:A37"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="A71:A79"/>
+    <mergeCell ref="B13:B23"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B39:B52"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2025-07-29 19:14:25 by tomori
</commit_message>
<xml_diff>
--- a/Instruction.xlsx
+++ b/Instruction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Lab\MATLAB Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C841C3-9A06-4861-B520-590B18E2C019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F63F92-2643-4760-AC92-BB305A2A520A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="251">
   <si>
     <t>data format conversion</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1011,6 +1011,30 @@
   </si>
   <si>
     <t>分组boxplot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mBoxplotGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>进阶版boxplotGroup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exportFigure2PDF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将figure导出为指定尺寸大小的pdf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kilosort4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kilosort4的matlab API接口，可以调用对应python脚本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1018,7 +1042,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,6 +1106,13 @@
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1181,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1226,6 +1257,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1235,10 +1267,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1250,10 +1285,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1534,10 +1566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1564,10 +1596,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1578,8 +1610,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="26"/>
-      <c r="B3" s="21"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="22"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1588,7 +1620,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="27"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="6" t="s">
         <v>30</v>
       </c>
@@ -1600,10 +1632,10 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="21" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1614,8 +1646,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="28"/>
-      <c r="B6" s="24"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="9" t="s">
         <v>123</v>
       </c>
@@ -1624,8 +1656,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="28"/>
-      <c r="B7" s="24"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="9" t="s">
         <v>124</v>
       </c>
@@ -1634,8 +1666,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="28"/>
-      <c r="B8" s="24"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="3" t="s">
         <v>212</v>
       </c>
@@ -1644,8 +1676,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="28"/>
-      <c r="B9" s="24"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="3" t="s">
         <v>187</v>
       </c>
@@ -1654,8 +1686,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="28"/>
-      <c r="B10" s="24"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="3" t="s">
         <v>214</v>
       </c>
@@ -1664,8 +1696,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="28"/>
-      <c r="B11" s="21"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="22"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1674,7 +1706,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6" t="s">
         <v>29</v>
       </c>
@@ -1686,8 +1718,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="28"/>
-      <c r="B13" s="20" t="s">
+      <c r="A13" s="24"/>
+      <c r="B13" s="21" t="s">
         <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1698,8 +1730,8 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="28"/>
-      <c r="B14" s="24"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="25"/>
       <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
@@ -1708,8 +1740,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="28"/>
-      <c r="B15" s="24"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="25"/>
       <c r="C15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1718,8 +1750,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="28"/>
-      <c r="B16" s="24"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="25"/>
       <c r="C16" s="3" t="s">
         <v>171</v>
       </c>
@@ -1728,8 +1760,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="24"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
       <c r="C17" s="3" t="s">
         <v>105</v>
       </c>
@@ -1738,8 +1770,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
-      <c r="B18" s="24"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="25"/>
       <c r="C18" s="9" t="s">
         <v>128</v>
       </c>
@@ -1748,8 +1780,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
-      <c r="B19" s="24"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="25"/>
       <c r="C19" s="9" t="s">
         <v>136</v>
       </c>
@@ -1758,8 +1790,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="28"/>
-      <c r="B20" s="24"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="25"/>
       <c r="C20" s="9" t="s">
         <v>132</v>
       </c>
@@ -1768,8 +1800,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
-      <c r="B21" s="24"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
       <c r="C21" s="9" t="s">
         <v>134</v>
       </c>
@@ -1778,8 +1810,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="28"/>
-      <c r="B22" s="24"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="25"/>
       <c r="C22" s="3" t="s">
         <v>130</v>
       </c>
@@ -1788,8 +1820,8 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="28"/>
-      <c r="B23" s="21"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="22"/>
       <c r="C23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1798,8 +1830,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="28"/>
-      <c r="B24" s="20" t="s">
+      <c r="A24" s="24"/>
+      <c r="B24" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1810,8 +1842,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="28"/>
-      <c r="B25" s="21"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="22"/>
       <c r="C25" s="2" t="s">
         <v>125</v>
       </c>
@@ -1820,8 +1852,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
-      <c r="B26" s="20" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="21" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1832,8 +1864,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="28"/>
-      <c r="B27" s="21"/>
+      <c r="A27" s="24"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="3" t="s">
         <v>34</v>
       </c>
@@ -1842,8 +1874,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
-      <c r="B28" s="20" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="21" t="s">
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1854,8 +1886,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="28"/>
-      <c r="B29" s="24"/>
+      <c r="A29" s="24"/>
+      <c r="B29" s="25"/>
       <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
@@ -1864,8 +1896,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
-      <c r="B30" s="24"/>
+      <c r="A30" s="24"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="2" t="s">
         <v>217</v>
       </c>
@@ -1874,8 +1906,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="28"/>
-      <c r="B31" s="24"/>
+      <c r="A31" s="24"/>
+      <c r="B31" s="25"/>
       <c r="C31" s="2" t="s">
         <v>118</v>
       </c>
@@ -1884,8 +1916,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="28"/>
-      <c r="B32" s="24"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="25"/>
       <c r="C32" s="2" t="s">
         <v>120</v>
       </c>
@@ -1894,8 +1926,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
-      <c r="B33" s="24"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="25"/>
       <c r="C33" s="2" t="s">
         <v>116</v>
       </c>
@@ -1904,8 +1936,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="28"/>
-      <c r="B34" s="24"/>
+      <c r="A34" s="24"/>
+      <c r="B34" s="25"/>
       <c r="C34" s="2" t="s">
         <v>114</v>
       </c>
@@ -1914,8 +1946,8 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
-      <c r="B35" s="24"/>
+      <c r="A35" s="24"/>
+      <c r="B35" s="25"/>
       <c r="C35" s="2" t="s">
         <v>218</v>
       </c>
@@ -1924,8 +1956,8 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="28"/>
-      <c r="B36" s="24"/>
+      <c r="A36" s="24"/>
+      <c r="B36" s="25"/>
       <c r="C36" s="2" t="s">
         <v>112</v>
       </c>
@@ -1934,8 +1966,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="21"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="22"/>
       <c r="C37" s="3" t="s">
         <v>40</v>
       </c>
@@ -1944,7 +1976,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="22" t="s">
+      <c r="A38" s="23" t="s">
         <v>42</v>
       </c>
       <c r="B38" s="19" t="s">
@@ -1958,8 +1990,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
-      <c r="B39" s="20" t="s">
+      <c r="A39" s="24"/>
+      <c r="B39" s="21" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -1970,8 +2002,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="28"/>
-      <c r="B40" s="24"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="25"/>
       <c r="C40" s="2" t="s">
         <v>46</v>
       </c>
@@ -1980,8 +2012,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="24"/>
+      <c r="B41" s="25"/>
       <c r="C41" s="2" t="s">
         <v>48</v>
       </c>
@@ -1990,8 +2022,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="28"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="25"/>
       <c r="C42" s="2" t="s">
         <v>155</v>
       </c>
@@ -2000,8 +2032,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="28"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="24"/>
+      <c r="B43" s="25"/>
       <c r="C43" s="2" t="s">
         <v>157</v>
       </c>
@@ -2010,8 +2042,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="28"/>
-      <c r="B44" s="24"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="25"/>
       <c r="C44" s="2" t="s">
         <v>159</v>
       </c>
@@ -2020,8 +2052,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="28"/>
-      <c r="B45" s="24"/>
+      <c r="A45" s="24"/>
+      <c r="B45" s="25"/>
       <c r="C45" s="2" t="s">
         <v>163</v>
       </c>
@@ -2030,8 +2062,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="28"/>
-      <c r="B46" s="24"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="25"/>
       <c r="C46" s="2" t="s">
         <v>165</v>
       </c>
@@ -2040,8 +2072,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="28"/>
-      <c r="B47" s="24"/>
+      <c r="A47" s="24"/>
+      <c r="B47" s="25"/>
       <c r="C47" s="2" t="s">
         <v>167</v>
       </c>
@@ -2050,8 +2082,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="28"/>
-      <c r="B48" s="24"/>
+      <c r="A48" s="24"/>
+      <c r="B48" s="25"/>
       <c r="C48" s="2" t="s">
         <v>169</v>
       </c>
@@ -2060,8 +2092,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="28"/>
-      <c r="B49" s="24"/>
+      <c r="A49" s="24"/>
+      <c r="B49" s="25"/>
       <c r="C49" s="3" t="s">
         <v>161</v>
       </c>
@@ -2070,8 +2102,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="28"/>
-      <c r="B50" s="24"/>
+      <c r="A50" s="24"/>
+      <c r="B50" s="25"/>
       <c r="C50" s="3" t="s">
         <v>184</v>
       </c>
@@ -2080,9 +2112,9 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="28"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="29" t="s">
+      <c r="A51" s="24"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="20" t="s">
         <v>223</v>
       </c>
       <c r="D51" s="2" t="s">
@@ -2090,8 +2122,8 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="28"/>
-      <c r="B52" s="21"/>
+      <c r="A52" s="24"/>
+      <c r="B52" s="22"/>
       <c r="C52" s="3" t="s">
         <v>50</v>
       </c>
@@ -2100,8 +2132,8 @@
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="28"/>
-      <c r="B53" s="20" t="s">
+      <c r="A53" s="24"/>
+      <c r="B53" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C53" s="16" t="s">
@@ -2112,8 +2144,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="28"/>
-      <c r="B54" s="24"/>
+      <c r="A54" s="24"/>
+      <c r="B54" s="25"/>
       <c r="C54" s="3" t="s">
         <v>182</v>
       </c>
@@ -2122,8 +2154,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="28"/>
-      <c r="B55" s="24"/>
+      <c r="A55" s="24"/>
+      <c r="B55" s="25"/>
       <c r="C55" s="16" t="s">
         <v>183</v>
       </c>
@@ -2132,8 +2164,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="28"/>
-      <c r="B56" s="21"/>
+      <c r="A56" s="24"/>
+      <c r="B56" s="22"/>
       <c r="C56" s="3" t="s">
         <v>54</v>
       </c>
@@ -2142,10 +2174,10 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="22" t="s">
+      <c r="A57" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="20"/>
+      <c r="B57" s="21"/>
       <c r="C57" s="3" t="s">
         <v>103</v>
       </c>
@@ -2154,8 +2186,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="28"/>
-      <c r="B58" s="24"/>
+      <c r="A58" s="24"/>
+      <c r="B58" s="25"/>
       <c r="C58" s="3" t="s">
         <v>108</v>
       </c>
@@ -2164,8 +2196,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="28"/>
-      <c r="B59" s="24"/>
+      <c r="A59" s="24"/>
+      <c r="B59" s="25"/>
       <c r="C59" s="3" t="s">
         <v>110</v>
       </c>
@@ -2174,8 +2206,8 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="28"/>
-      <c r="B60" s="24"/>
+      <c r="A60" s="24"/>
+      <c r="B60" s="25"/>
       <c r="C60" s="2" t="s">
         <v>57</v>
       </c>
@@ -2184,8 +2216,8 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="28"/>
-      <c r="B61" s="24"/>
+      <c r="A61" s="24"/>
+      <c r="B61" s="25"/>
       <c r="C61" s="2" t="s">
         <v>173</v>
       </c>
@@ -2194,8 +2226,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="28"/>
-      <c r="B62" s="24"/>
+      <c r="A62" s="24"/>
+      <c r="B62" s="25"/>
       <c r="C62" s="3" t="s">
         <v>174</v>
       </c>
@@ -2204,8 +2236,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="28"/>
-      <c r="B63" s="24"/>
+      <c r="A63" s="24"/>
+      <c r="B63" s="25"/>
       <c r="C63" s="2" t="s">
         <v>59</v>
       </c>
@@ -2214,8 +2246,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="28"/>
-      <c r="B64" s="24"/>
+      <c r="A64" s="24"/>
+      <c r="B64" s="25"/>
       <c r="C64" s="2" t="s">
         <v>60</v>
       </c>
@@ -2224,8 +2256,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="28"/>
-      <c r="B65" s="24"/>
+      <c r="A65" s="24"/>
+      <c r="B65" s="25"/>
       <c r="C65" s="2" t="s">
         <v>61</v>
       </c>
@@ -2234,8 +2266,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="28"/>
-      <c r="B66" s="24"/>
+      <c r="A66" s="24"/>
+      <c r="B66" s="25"/>
       <c r="C66" s="3" t="s">
         <v>63</v>
       </c>
@@ -2244,8 +2276,8 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="28"/>
-      <c r="B67" s="24"/>
+      <c r="A67" s="24"/>
+      <c r="B67" s="25"/>
       <c r="C67" s="3" t="s">
         <v>65</v>
       </c>
@@ -2254,8 +2286,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="28"/>
-      <c r="B68" s="24"/>
+      <c r="A68" s="24"/>
+      <c r="B68" s="25"/>
       <c r="C68" s="3" t="s">
         <v>227</v>
       </c>
@@ -2264,471 +2296,501 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="28"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="9" t="s">
+      <c r="A69" s="24"/>
+      <c r="B69" s="25"/>
+      <c r="C69" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="24"/>
+      <c r="B70" s="25"/>
+      <c r="C70" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="21"/>
-      <c r="C70" s="3" t="s">
+    <row r="71" spans="1:4" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="26"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="22" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B72" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="28"/>
-      <c r="B72" s="20" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="24"/>
+      <c r="B73" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="2" t="s">
+      <c r="C73" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D73" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="28"/>
-      <c r="B73" s="21"/>
-      <c r="C73" s="2" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="24"/>
+      <c r="B74" s="25"/>
+      <c r="C74" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="24"/>
+      <c r="B75" s="22"/>
+      <c r="C75" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D75" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="28"/>
-      <c r="B74" s="20" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="24"/>
+      <c r="B76" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="D76" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="28"/>
-      <c r="B75" s="21"/>
-      <c r="C75" s="2" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="24"/>
+      <c r="B77" s="22"/>
+      <c r="C77" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="28"/>
-      <c r="B76" s="20" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="24"/>
+      <c r="B78" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C76" s="3" t="s">
+      <c r="C78" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="28"/>
-      <c r="B77" s="24"/>
-      <c r="C77" s="2" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="24"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="28"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="2" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="24"/>
+      <c r="B80" s="25"/>
+      <c r="C80" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="D80" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="23"/>
-      <c r="B79" s="21"/>
-      <c r="C79" s="2" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="26"/>
+      <c r="B81" s="22"/>
+      <c r="C81" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D81" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="22" t="s">
+    <row r="82" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="3" t="s">
+      <c r="B82" s="21"/>
+      <c r="C82" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D80" s="2" t="s">
+      <c r="D82" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="28"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="9" t="s">
+    <row r="83" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="24"/>
+      <c r="B83" s="25"/>
+      <c r="C83" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="D81" s="2" t="s">
+      <c r="D83" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="28"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="2" t="s">
+    <row r="84" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="24"/>
+      <c r="B84" s="25"/>
+      <c r="C84" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D84" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="28"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="10" t="s">
+    <row r="85" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="24"/>
+      <c r="B85" s="25"/>
+      <c r="C85" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="D85" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="28"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="3" t="s">
+    <row r="86" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="24"/>
+      <c r="B86" s="25"/>
+      <c r="C86" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="D86" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="28"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="3" t="s">
+    <row r="87" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="24"/>
+      <c r="B87" s="25"/>
+      <c r="C87" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="28"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="2" t="s">
+    <row r="88" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="24"/>
+      <c r="B88" s="25"/>
+      <c r="C88" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="D88" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="28"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="2" t="s">
+    <row r="89" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="24"/>
+      <c r="B89" s="25"/>
+      <c r="C89" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="D89" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="28"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="3" t="s">
+    <row r="90" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="24"/>
+      <c r="B90" s="25"/>
+      <c r="C90" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D88" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="28"/>
-      <c r="B89" s="24"/>
-      <c r="C89" s="3" t="s">
+    <row r="91" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="24"/>
+      <c r="B91" s="25"/>
+      <c r="C91" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="D89" s="2" t="s">
+      <c r="D91" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="28"/>
-      <c r="B90" s="24"/>
-      <c r="C90" s="2" t="s">
+    <row r="92" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="24"/>
+      <c r="B92" s="25"/>
+      <c r="C92" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="28"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="2" t="s">
+    <row r="93" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="24"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="28"/>
-      <c r="B92" s="24"/>
-      <c r="C92" s="2" t="s">
+    <row r="94" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="24"/>
+      <c r="B94" s="25"/>
+      <c r="C94" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="28"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="2" t="s">
+    <row r="95" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="24"/>
+      <c r="B95" s="25"/>
+      <c r="C95" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="28"/>
-      <c r="B94" s="24"/>
-      <c r="C94" s="2" t="s">
+    <row r="96" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="24"/>
+      <c r="B96" s="25"/>
+      <c r="C96" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="28"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="2" t="s">
+    <row r="97" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="24"/>
+      <c r="B97" s="25"/>
+      <c r="C97" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="28"/>
-      <c r="B96" s="24"/>
-      <c r="C96" s="2" t="s">
+    <row r="98" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="24"/>
+      <c r="B98" s="25"/>
+      <c r="C98" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="28"/>
-      <c r="B97" s="24"/>
-      <c r="C97" s="2" t="s">
+    <row r="99" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="24"/>
+      <c r="B99" s="25"/>
+      <c r="C99" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D99" s="2" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="28"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="2" t="s">
+    <row r="100" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="24"/>
+      <c r="B100" s="25"/>
+      <c r="C100" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="D100" s="2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="28"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="2" t="s">
+    <row r="101" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="24"/>
+      <c r="B101" s="25"/>
+      <c r="C101" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="28"/>
-      <c r="B100" s="24"/>
-      <c r="C100" s="2" t="s">
+    <row r="102" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="24"/>
+      <c r="B102" s="25"/>
+      <c r="C102" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D100" s="2" t="s">
+      <c r="D102" s="2" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="28"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="2" t="s">
+    <row r="103" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="24"/>
+      <c r="B103" s="25"/>
+      <c r="C103" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="D103" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="28"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="2" t="s">
+    <row r="104" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="24"/>
+      <c r="B104" s="25"/>
+      <c r="C104" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="D104" s="2" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="28"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="2" t="s">
+    <row r="105" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="24"/>
+      <c r="B105" s="25"/>
+      <c r="C105" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D103" s="2" t="s">
+      <c r="D105" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="28"/>
-      <c r="B104" s="24"/>
-      <c r="C104" s="2" t="s">
+    <row r="106" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="24"/>
+      <c r="B106" s="25"/>
+      <c r="C106" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D104" s="2" t="s">
+      <c r="D106" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="28"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="3" t="s">
+    <row r="107" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="24"/>
+      <c r="B107" s="25"/>
+      <c r="C107" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D105" s="2" t="s">
+      <c r="D107" s="2" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="23"/>
-      <c r="B106" s="21"/>
-      <c r="C106" s="3" t="s">
+    <row r="108" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="24"/>
+      <c r="B108" s="25"/>
+      <c r="C108" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="D106" s="2" t="s">
+      <c r="D108" s="2" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="22" t="s">
+    <row r="109" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="26"/>
+      <c r="B109" s="22"/>
+      <c r="C109" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="B107" s="20" t="s">
+      <c r="B110" s="21" t="s">
         <v>207</v>
       </c>
-      <c r="C107" s="2" t="s">
+      <c r="C110" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D107" s="2" t="s">
+      <c r="D110" s="2" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" s="23"/>
-      <c r="B108" s="21"/>
-      <c r="C108" s="2" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="26"/>
+      <c r="B111" s="22"/>
+      <c r="C111" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="D108" s="2" t="s">
+      <c r="D111" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="18"/>
-      <c r="B109" s="17"/>
-    </row>
-    <row r="110" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="13" t="s">
+    <row r="112" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A112" s="18"/>
+      <c r="B112" s="17"/>
+    </row>
+    <row r="113" spans="1:2" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A113" s="13" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="14"/>
-      <c r="B111" s="12" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" s="14"/>
+      <c r="B114" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" s="11"/>
-      <c r="B112" s="12" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="11"/>
+      <c r="B115" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="15"/>
-      <c r="B113" s="12" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="15"/>
+      <c r="B116" s="12" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A38:A56"/>
-    <mergeCell ref="B80:B106"/>
-    <mergeCell ref="A80:A106"/>
-    <mergeCell ref="B53:B56"/>
-    <mergeCell ref="A57:A70"/>
-    <mergeCell ref="B57:B70"/>
-    <mergeCell ref="B107:B108"/>
-    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="A110:A111"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A37"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="A71:A79"/>
+    <mergeCell ref="A72:A81"/>
     <mergeCell ref="B13:B23"/>
     <mergeCell ref="B28:B37"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B76:B79"/>
+    <mergeCell ref="B73:B75"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B81"/>
     <mergeCell ref="B39:B52"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A38:A56"/>
+    <mergeCell ref="B82:B109"/>
+    <mergeCell ref="A82:A109"/>
+    <mergeCell ref="B53:B56"/>
+    <mergeCell ref="A57:A71"/>
+    <mergeCell ref="B57:B71"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>